<commit_message>
updated aac, bl, kb, bm models
</commit_message>
<xml_diff>
--- a/bolser-lewis/source/bolser-lewis.xlsx
+++ b/bolser-lewis/source/bolser-lewis.xlsx
@@ -44,44 +44,6 @@
 </t>
       </text>
     </comment>
-    <comment authorId="0" ref="C80">
-      <text>
-        <t xml:space="preserve">http://purl.obolibrary.org/obo/UBERON_0000379
-aka
-http://uri.interlex.org/ilx_0724678
-	-Tom Gillespie
-+troysincomb@gmail.com
-	-Tom Gillespie
-Thumbs up for merge.
-	-Tom Gillespie
-👍
-	-Troy</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="C74">
-      <text>
-        <t xml:space="preserve">Is http://purl.obolibrary.org/obo/UBERON_0009050 the correct id here? Aka http://uri.interlex.org/base/ilx_0110729. If so we will merge the terms.
-	-Tom Gillespie
-+troysincomb@gmail.com
-	-Tom Gillespie
-Thumbs up for merge.
-	-Tom Gillespie
-👍
-	-Troy</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="C38">
-      <text>
-        <t xml:space="preserve">http://purl.org/sig/ont/fma/fma14056 is White communicating ramus of thoracic ventral ramus and doesn't specify T1.  Added to Interlex: http://uri.interlex.org/base/ilx_0738372
-	-M Martone</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="C33">
-      <text>
-        <t xml:space="preserve">According to FMA, this identifier only points to Rexed Lamina VII not Rexed Lamina VII of T1.  So I have created the cross product in Interlex: http://uri.interlex.org/base/ilx_0738371
-	-M Martone</t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -120,7 +82,7 @@
     <t>bolser-lewis</t>
   </si>
   <si>
-    <t>Bolser-Lewis map</t>
+    <t>Bolser-Lewis Model of the Physiology of the Superior Cervical Ganglion</t>
   </si>
   <si>
     <t>bolew</t>

</xml_diff>